<commit_message>
Actualización automática: 2026-02-05 11:36:15
</commit_message>
<xml_diff>
--- a/Elastic_Agent_SIEM/Salidas_Playbooks/elastic_agent_report.xlsx
+++ b/Elastic_Agent_SIEM/Salidas_Playbooks/elastic_agent_report.xlsx
@@ -449,7 +449,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -531,17 +531,17 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>CRM04_K8S</t>
+          <t>APBOGDISMANTIS</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>crm04_k8s</t>
+          <t>mantis-new</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>10.181.4.11</t>
+          <t>10.181.5.68</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr">
@@ -637,6 +637,1203 @@
         </is>
       </c>
       <c r="K3" s="4" t="inlineStr">
+        <is>
+          <t>Acción ejecutada: RE-ENROLL (sin validación de servicio)</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>MICROSERVICIOS04_1</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>k4</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>10.181.3.183</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="F4" s="3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G4" s="4" t="inlineStr">
+        <is>
+          <t>Successfully enrolled the Elastic Agent.</t>
+        </is>
+      </c>
+      <c r="H4" s="5" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I4" s="5" t="inlineStr">
+        <is>
+          <t>NO VALIDADO</t>
+        </is>
+      </c>
+      <c r="J4" s="5" t="inlineStr">
+        <is>
+          <t>NO OK</t>
+        </is>
+      </c>
+      <c r="K4" s="4" t="inlineStr">
+        <is>
+          <t>Acción ejecutada: RE-ENROLL (sin validación de servicio)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>LPBOGDIS01</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>crm05_k8s</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>10.181.4.16</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="F5" s="3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G5" s="4" t="inlineStr">
+        <is>
+          <t>Successfully enrolled the Elastic Agent.</t>
+        </is>
+      </c>
+      <c r="H5" s="5" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I5" s="5" t="inlineStr">
+        <is>
+          <t>NO VALIDADO</t>
+        </is>
+      </c>
+      <c r="J5" s="5" t="inlineStr">
+        <is>
+          <t>NO OK</t>
+        </is>
+      </c>
+      <c r="K5" s="4" t="inlineStr">
+        <is>
+          <t>Acción ejecutada: RE-ENROLL (sin validación de servicio)</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>MICROCRMBOGDIS2</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>microscrm_new</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>10.181.5.126</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="F6" s="3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G6" s="4" t="inlineStr">
+        <is>
+          <t>Successfully enrolled the Elastic Agent.</t>
+        </is>
+      </c>
+      <c r="H6" s="5" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I6" s="5" t="inlineStr">
+        <is>
+          <t>NO VALIDADO</t>
+        </is>
+      </c>
+      <c r="J6" s="5" t="inlineStr">
+        <is>
+          <t>NO OK</t>
+        </is>
+      </c>
+      <c r="K6" s="4" t="inlineStr">
+        <is>
+          <t>Acción ejecutada: RE-ENROLL (sin validación de servicio)</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>CONTACTCRMDBBOGDIS01</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>contactcrmdbprd</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>10.181.5.214</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="F7" s="3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G7" s="4" t="inlineStr">
+        <is>
+          <t>Successfully enrolled the Elastic Agent.</t>
+        </is>
+      </c>
+      <c r="H7" s="5" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I7" s="5" t="inlineStr">
+        <is>
+          <t>NO VALIDADO</t>
+        </is>
+      </c>
+      <c r="J7" s="5" t="inlineStr">
+        <is>
+          <t>NO OK</t>
+        </is>
+      </c>
+      <c r="K7" s="4" t="inlineStr">
+        <is>
+          <t>Acción ejecutada: RE-ENROLL (sin validación de servicio)</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>vm-eu2-appdru03-rst</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>VM-EU2-APPDRU03-RST</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>10.0.16.149</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E8" s="2" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="F8" s="3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G8" s="4" t="inlineStr">
+        <is>
+          <t>Successfully enrolled the Elastic Agent.</t>
+        </is>
+      </c>
+      <c r="H8" s="5" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I8" s="5" t="inlineStr">
+        <is>
+          <t>NO VALIDADO</t>
+        </is>
+      </c>
+      <c r="J8" s="5" t="inlineStr">
+        <is>
+          <t>NO OK</t>
+        </is>
+      </c>
+      <c r="K8" s="4" t="inlineStr">
+        <is>
+          <t>Acción ejecutada: RE-ENROLL (sin validación de servicio)</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>alkexadbadm02vm4</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>alkexadbadm02vm4</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
+          <t>192.168.97.54</t>
+        </is>
+      </c>
+      <c r="D9" s="2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="F9" s="3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G9" s="4" t="inlineStr">
+        <is>
+          <t>Successfully enrolled the Elastic Agent.</t>
+        </is>
+      </c>
+      <c r="H9" s="5" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I9" s="5" t="inlineStr">
+        <is>
+          <t>NO VALIDADO</t>
+        </is>
+      </c>
+      <c r="J9" s="5" t="inlineStr">
+        <is>
+          <t>NO OK</t>
+        </is>
+      </c>
+      <c r="K9" s="4" t="inlineStr">
+        <is>
+          <t>Acción ejecutada: RE-ENROLL (sin validación de servicio)</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>alkexadbadm01vm4</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>alkexadbadm01vm4</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>192.168.97.53</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="F10" s="3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G10" s="4" t="inlineStr">
+        <is>
+          <t>Successfully enrolled the Elastic Agent.</t>
+        </is>
+      </c>
+      <c r="H10" s="5" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I10" s="5" t="inlineStr">
+        <is>
+          <t>NO VALIDADO</t>
+        </is>
+      </c>
+      <c r="J10" s="5" t="inlineStr">
+        <is>
+          <t>NO OK</t>
+        </is>
+      </c>
+      <c r="K10" s="4" t="inlineStr">
+        <is>
+          <t>Acción ejecutada: RE-ENROLL (sin validación de servicio)</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>alkexadbadm02vm2</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>alkexadbadm02vm2</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>192.168.97.46</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="F11" s="3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G11" s="4" t="inlineStr">
+        <is>
+          <t>Successfully enrolled the Elastic Agent.</t>
+        </is>
+      </c>
+      <c r="H11" s="5" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I11" s="5" t="inlineStr">
+        <is>
+          <t>NO VALIDADO</t>
+        </is>
+      </c>
+      <c r="J11" s="5" t="inlineStr">
+        <is>
+          <t>NO OK</t>
+        </is>
+      </c>
+      <c r="K11" s="4" t="inlineStr">
+        <is>
+          <t>Acción ejecutada: RE-ENROLL (sin validación de servicio)</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>alkexadbadm01vm2</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>alkexadbadm01vm2</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
+        <is>
+          <t>192.168.97.45</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="F12" s="3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G12" s="4" t="inlineStr">
+        <is>
+          <t>Successfully enrolled the Elastic Agent.</t>
+        </is>
+      </c>
+      <c r="H12" s="5" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I12" s="5" t="inlineStr">
+        <is>
+          <t>NO VALIDADO</t>
+        </is>
+      </c>
+      <c r="J12" s="5" t="inlineStr">
+        <is>
+          <t>NO OK</t>
+        </is>
+      </c>
+      <c r="K12" s="4" t="inlineStr">
+        <is>
+          <t>Acción ejecutada: RE-ENROLL (sin validación de servicio)</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>alkexadbadm04vm1</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="inlineStr">
+        <is>
+          <t>alkexadbadm04vm1</t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="inlineStr">
+        <is>
+          <t>192.168.97.44</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="F13" s="3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G13" s="4" t="inlineStr">
+        <is>
+          <t>Successfully enrolled the Elastic Agent.</t>
+        </is>
+      </c>
+      <c r="H13" s="5" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I13" s="5" t="inlineStr">
+        <is>
+          <t>NO VALIDADO</t>
+        </is>
+      </c>
+      <c r="J13" s="5" t="inlineStr">
+        <is>
+          <t>NO OK</t>
+        </is>
+      </c>
+      <c r="K13" s="4" t="inlineStr">
+        <is>
+          <t>Acción ejecutada: RE-ENROLL (sin validación de servicio)</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>alkexadbadm03vm1</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>alkexadbadm03vm1</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="inlineStr">
+        <is>
+          <t>192.168.97.43</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="F14" s="3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G14" s="4" t="inlineStr">
+        <is>
+          <t>Successfully enrolled the Elastic Agent.</t>
+        </is>
+      </c>
+      <c r="H14" s="5" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I14" s="5" t="inlineStr">
+        <is>
+          <t>NO VALIDADO</t>
+        </is>
+      </c>
+      <c r="J14" s="5" t="inlineStr">
+        <is>
+          <t>NO OK</t>
+        </is>
+      </c>
+      <c r="K14" s="4" t="inlineStr">
+        <is>
+          <t>Acción ejecutada: RE-ENROLL (sin validación de servicio)</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>alkexadbadm02vm1</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>alkexadbadm02vm1</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="inlineStr">
+        <is>
+          <t>192.168.97.42</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="F15" s="3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G15" s="4" t="inlineStr">
+        <is>
+          <t>Successfully enrolled the Elastic Agent.</t>
+        </is>
+      </c>
+      <c r="H15" s="5" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I15" s="5" t="inlineStr">
+        <is>
+          <t>NO VALIDADO</t>
+        </is>
+      </c>
+      <c r="J15" s="5" t="inlineStr">
+        <is>
+          <t>NO OK</t>
+        </is>
+      </c>
+      <c r="K15" s="4" t="inlineStr">
+        <is>
+          <t>Acción ejecutada: RE-ENROLL (sin validación de servicio)</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>BATMAN</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="inlineStr">
+        <is>
+          <t>batman</t>
+        </is>
+      </c>
+      <c r="C16" s="2" t="inlineStr">
+        <is>
+          <t>10.181.3.25</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="F16" s="3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G16" s="4" t="inlineStr">
+        <is>
+          <t>Successfully enrolled the Elastic Agent.</t>
+        </is>
+      </c>
+      <c r="H16" s="5" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I16" s="5" t="inlineStr">
+        <is>
+          <t>NO VALIDADO</t>
+        </is>
+      </c>
+      <c r="J16" s="5" t="inlineStr">
+        <is>
+          <t>NO OK</t>
+        </is>
+      </c>
+      <c r="K16" s="4" t="inlineStr">
+        <is>
+          <t>Acción ejecutada: RE-ENROLL (sin validación de servicio)</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>BATMAN_NEW</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="inlineStr">
+        <is>
+          <t>batman_new</t>
+        </is>
+      </c>
+      <c r="C17" s="2" t="inlineStr">
+        <is>
+          <t>10.181.5.224</t>
+        </is>
+      </c>
+      <c r="D17" s="2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="F17" s="3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G17" s="4" t="inlineStr">
+        <is>
+          <t>Successfully enrolled the Elastic Agent.</t>
+        </is>
+      </c>
+      <c r="H17" s="5" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I17" s="5" t="inlineStr">
+        <is>
+          <t>NO VALIDADO</t>
+        </is>
+      </c>
+      <c r="J17" s="5" t="inlineStr">
+        <is>
+          <t>NO OK</t>
+        </is>
+      </c>
+      <c r="K17" s="4" t="inlineStr">
+        <is>
+          <t>Acción ejecutada: RE-ENROLL (sin validación de servicio)</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>geopos-fx-n1</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="inlineStr">
+        <is>
+          <t>geopos-fx-n1</t>
+        </is>
+      </c>
+      <c r="C18" s="2" t="inlineStr">
+        <is>
+          <t>10.181.0.113</t>
+        </is>
+      </c>
+      <c r="D18" s="2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E18" s="2" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="F18" s="3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G18" s="4" t="inlineStr">
+        <is>
+          <t>Successfully enrolled the Elastic Agent.</t>
+        </is>
+      </c>
+      <c r="H18" s="5" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I18" s="5" t="inlineStr">
+        <is>
+          <t>NO VALIDADO</t>
+        </is>
+      </c>
+      <c r="J18" s="5" t="inlineStr">
+        <is>
+          <t>NO OK</t>
+        </is>
+      </c>
+      <c r="K18" s="4" t="inlineStr">
+        <is>
+          <t>Acción ejecutada: RE-ENROLL (sin validación de servicio)</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="inlineStr">
+        <is>
+          <t>geopos-fx-n2</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="inlineStr">
+        <is>
+          <t>geopos-fx-n2</t>
+        </is>
+      </c>
+      <c r="C19" s="2" t="inlineStr">
+        <is>
+          <t>10.181.0.117</t>
+        </is>
+      </c>
+      <c r="D19" s="2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E19" s="2" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="F19" s="3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G19" s="4" t="inlineStr">
+        <is>
+          <t>Successfully enrolled the Elastic Agent.</t>
+        </is>
+      </c>
+      <c r="H19" s="5" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I19" s="5" t="inlineStr">
+        <is>
+          <t>NO VALIDADO</t>
+        </is>
+      </c>
+      <c r="J19" s="5" t="inlineStr">
+        <is>
+          <t>NO OK</t>
+        </is>
+      </c>
+      <c r="K19" s="4" t="inlineStr">
+        <is>
+          <t>Acción ejecutada: RE-ENROLL (sin validación de servicio)</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>CRM_FILE</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="inlineStr">
+        <is>
+          <t>crm-file</t>
+        </is>
+      </c>
+      <c r="C20" s="2" t="inlineStr">
+        <is>
+          <t>10.181.3.36</t>
+        </is>
+      </c>
+      <c r="D20" s="2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E20" s="2" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="F20" s="3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G20" s="4" t="inlineStr">
+        <is>
+          <t>Successfully enrolled the Elastic Agent.</t>
+        </is>
+      </c>
+      <c r="H20" s="5" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I20" s="5" t="inlineStr">
+        <is>
+          <t>NO VALIDADO</t>
+        </is>
+      </c>
+      <c r="J20" s="5" t="inlineStr">
+        <is>
+          <t>NO OK</t>
+        </is>
+      </c>
+      <c r="K20" s="4" t="inlineStr">
+        <is>
+          <t>Acción ejecutada: RE-ENROLL (sin validación de servicio)</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="inlineStr">
+        <is>
+          <t>DESPACHOS03</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="inlineStr">
+        <is>
+          <t>tobin_new</t>
+        </is>
+      </c>
+      <c r="C21" s="2" t="inlineStr">
+        <is>
+          <t>10.181.3.106</t>
+        </is>
+      </c>
+      <c r="D21" s="2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E21" s="2" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="F21" s="3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G21" s="4" t="inlineStr">
+        <is>
+          <t>Successfully enrolled the Elastic Agent.</t>
+        </is>
+      </c>
+      <c r="H21" s="5" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I21" s="5" t="inlineStr">
+        <is>
+          <t>NO VALIDADO</t>
+        </is>
+      </c>
+      <c r="J21" s="5" t="inlineStr">
+        <is>
+          <t>NO OK</t>
+        </is>
+      </c>
+      <c r="K21" s="4" t="inlineStr">
+        <is>
+          <t>Acción ejecutada: RE-ENROLL (sin validación de servicio)</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>mon_zabbix_proxy</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="inlineStr">
+        <is>
+          <t>mon_zabbix_proxy</t>
+        </is>
+      </c>
+      <c r="C22" s="2" t="inlineStr">
+        <is>
+          <t>10.181.5.210</t>
+        </is>
+      </c>
+      <c r="D22" s="2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E22" s="2" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="F22" s="3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G22" s="4" t="inlineStr">
+        <is>
+          <t>Successfully enrolled the Elastic Agent.</t>
+        </is>
+      </c>
+      <c r="H22" s="5" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I22" s="5" t="inlineStr">
+        <is>
+          <t>NO VALIDADO</t>
+        </is>
+      </c>
+      <c r="J22" s="5" t="inlineStr">
+        <is>
+          <t>NO OK</t>
+        </is>
+      </c>
+      <c r="K22" s="4" t="inlineStr">
+        <is>
+          <t>Acción ejecutada: RE-ENROLL (sin validación de servicio)</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="inlineStr">
+        <is>
+          <t>crm_db3</t>
+        </is>
+      </c>
+      <c r="B23" s="2" t="inlineStr">
+        <is>
+          <t>crm_db3</t>
+        </is>
+      </c>
+      <c r="C23" s="2" t="inlineStr">
+        <is>
+          <t>10.181.4.103</t>
+        </is>
+      </c>
+      <c r="D23" s="2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E23" s="2" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="F23" s="3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G23" s="4" t="inlineStr">
+        <is>
+          <t>Successfully enrolled the Elastic Agent.</t>
+        </is>
+      </c>
+      <c r="H23" s="5" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I23" s="5" t="inlineStr">
+        <is>
+          <t>NO VALIDADO</t>
+        </is>
+      </c>
+      <c r="J23" s="5" t="inlineStr">
+        <is>
+          <t>NO OK</t>
+        </is>
+      </c>
+      <c r="K23" s="4" t="inlineStr">
+        <is>
+          <t>Acción ejecutada: RE-ENROLL (sin validación de servicio)</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="inlineStr">
+        <is>
+          <t>corbemovil__test</t>
+        </is>
+      </c>
+      <c r="B24" s="2" t="inlineStr">
+        <is>
+          <t>corbemovil__test</t>
+        </is>
+      </c>
+      <c r="C24" s="2" t="inlineStr">
+        <is>
+          <t>10.181.11.10</t>
+        </is>
+      </c>
+      <c r="D24" s="2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E24" s="2" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="F24" s="3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G24" s="4" t="inlineStr">
+        <is>
+          <t>Successfully enrolled the Elastic Agent.</t>
+        </is>
+      </c>
+      <c r="H24" s="5" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I24" s="5" t="inlineStr">
+        <is>
+          <t>NO VALIDADO</t>
+        </is>
+      </c>
+      <c r="J24" s="5" t="inlineStr">
+        <is>
+          <t>NO OK</t>
+        </is>
+      </c>
+      <c r="K24" s="4" t="inlineStr">
         <is>
           <t>Acción ejecutada: RE-ENROLL (sin validación de servicio)</t>
         </is>

</xml_diff>